<commit_message>
add orderofoperation.xlsx for lesson 19
</commit_message>
<xml_diff>
--- a/13. Monthly Budget.xlsx
+++ b/13. Monthly Budget.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\moin\Excel Practice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA5ECF39-08FD-4BB5-AB4B-2B2902A44BB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1DF3D26-6576-4E02-9371-B7A6E78175F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0525C57C-F6D3-4E5A-BABF-0921013F3FE3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{0525C57C-F6D3-4E5A-BABF-0921013F3FE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Monthly Budget " sheetId="3" r:id="rId1"/>
+    <sheet name="Monthly Budget  (2)" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="8">
   <si>
     <t>Bills</t>
   </si>
@@ -58,6 +59,9 @@
   <si>
     <t>Total</t>
   </si>
+  <si>
+    <t>Percent</t>
+  </si>
 </sst>
 </file>
 
@@ -67,7 +71,14 @@
     <numFmt numFmtId="166" formatCode="mmm/yyyy"/>
     <numFmt numFmtId="169" formatCode="mmm/dd/ddd/yyyy/mmm"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -101,29 +112,37 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -435,10 +454,240 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FF16D73-07B9-460A-92EB-0A055A3AA27D}">
+  <dimension ref="A2:O8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="11.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="1"/>
+    <col min="7" max="7" width="16.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:15" s="2" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4">
+        <v>44562</v>
+      </c>
+      <c r="C2" s="4">
+        <v>44593</v>
+      </c>
+      <c r="D2" s="4">
+        <v>44621</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" spans="1:15" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1000</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1000</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E3" s="2">
+        <f>SUM(B3:D3)</f>
+        <v>3000</v>
+      </c>
+      <c r="F3" s="1">
+        <f>E3/E$8</f>
+        <v>0.58536585365853655</v>
+      </c>
+      <c r="G3" s="5"/>
+    </row>
+    <row r="4" spans="1:15" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>125</v>
+      </c>
+      <c r="C4" s="1">
+        <v>125</v>
+      </c>
+      <c r="D4" s="1">
+        <v>100</v>
+      </c>
+      <c r="E4" s="2">
+        <f t="shared" ref="E4:E8" si="0">SUM(B4:D4)</f>
+        <v>350</v>
+      </c>
+      <c r="F4" s="1">
+        <f t="shared" ref="F4:F7" si="1">E4/E$8</f>
+        <v>6.8292682926829273E-2</v>
+      </c>
+      <c r="I4" s="1">
+        <v>10</v>
+      </c>
+      <c r="J4" s="1">
+        <v>20</v>
+      </c>
+      <c r="M4" s="1">
+        <v>5</v>
+      </c>
+      <c r="N4" s="1">
+        <f>I$4*$M4</f>
+        <v>50</v>
+      </c>
+      <c r="O4" s="1">
+        <f>J$4*$M4</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
+        <v>150</v>
+      </c>
+      <c r="C5" s="1">
+        <v>200</v>
+      </c>
+      <c r="D5" s="1">
+        <v>175</v>
+      </c>
+      <c r="E5" s="2">
+        <f t="shared" si="0"/>
+        <v>525</v>
+      </c>
+      <c r="F5" s="1">
+        <f t="shared" si="1"/>
+        <v>0.1024390243902439</v>
+      </c>
+      <c r="M5" s="1">
+        <v>6</v>
+      </c>
+      <c r="N5" s="1">
+        <f t="shared" ref="N5:N7" si="2">I$4*$M5</f>
+        <v>60</v>
+      </c>
+      <c r="O5" s="1">
+        <f>J$4*$M5</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1">
+        <v>300</v>
+      </c>
+      <c r="C6" s="1">
+        <v>275</v>
+      </c>
+      <c r="D6" s="1">
+        <v>350</v>
+      </c>
+      <c r="E6" s="2">
+        <f t="shared" si="0"/>
+        <v>925</v>
+      </c>
+      <c r="F6" s="1">
+        <f t="shared" si="1"/>
+        <v>0.18048780487804877</v>
+      </c>
+      <c r="M6" s="1">
+        <v>7</v>
+      </c>
+      <c r="N6" s="1">
+        <f t="shared" si="2"/>
+        <v>70</v>
+      </c>
+      <c r="O6" s="1">
+        <f>J$4*$M6</f>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1">
+        <v>100</v>
+      </c>
+      <c r="C7" s="1">
+        <v>100</v>
+      </c>
+      <c r="D7" s="1">
+        <v>125</v>
+      </c>
+      <c r="E7" s="2">
+        <f t="shared" si="0"/>
+        <v>325</v>
+      </c>
+      <c r="F7" s="1">
+        <f t="shared" si="1"/>
+        <v>6.3414634146341464E-2</v>
+      </c>
+      <c r="M7" s="1">
+        <v>8</v>
+      </c>
+      <c r="N7" s="1">
+        <f t="shared" si="2"/>
+        <v>80</v>
+      </c>
+      <c r="O7" s="1">
+        <f>J$4*$M7</f>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2">
+        <f>SUM(B3:B7)</f>
+        <v>1675</v>
+      </c>
+      <c r="C8" s="2">
+        <f>SUM(C3:C7)</f>
+        <v>1700</v>
+      </c>
+      <c r="D8" s="2">
+        <f>SUM(D3:D7)</f>
+        <v>1750</v>
+      </c>
+      <c r="E8" s="2">
+        <f t="shared" si="0"/>
+        <v>5125</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="B8:D8" formulaRange="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C79055A-5DDB-4DD7-8258-797C0A05ECC1}">
   <dimension ref="A2:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="I2" sqref="I2:Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -467,6 +716,9 @@
       <c r="E2" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="F2" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="G2" s="3"/>
     </row>
     <row r="3" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -486,6 +738,10 @@
         <f>SUM(B3:D3)</f>
         <v>3000</v>
       </c>
+      <c r="F3" s="6">
+        <f>E3/$E$8</f>
+        <v>0.58536585365853655</v>
+      </c>
       <c r="G3" s="5"/>
     </row>
     <row r="4" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -493,7 +749,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="C4" s="1">
         <v>125</v>
@@ -502,8 +758,12 @@
         <v>100</v>
       </c>
       <c r="E4" s="2">
-        <f t="shared" ref="E4:E7" si="0">SUM(B4:D4)</f>
-        <v>325</v>
+        <f t="shared" ref="E4:E8" si="0">SUM(B4:D4)</f>
+        <v>350</v>
+      </c>
+      <c r="F4" s="6">
+        <f t="shared" ref="F4:F7" si="1">E4/$E$8</f>
+        <v>6.8292682926829273E-2</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -523,6 +783,10 @@
         <f t="shared" si="0"/>
         <v>525</v>
       </c>
+      <c r="F5" s="6">
+        <f t="shared" si="1"/>
+        <v>0.1024390243902439</v>
+      </c>
     </row>
     <row r="6" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
@@ -535,11 +799,15 @@
         <v>275</v>
       </c>
       <c r="D6" s="1">
-        <v>150</v>
+        <v>350</v>
       </c>
       <c r="E6" s="2">
         <f t="shared" si="0"/>
-        <v>725</v>
+        <v>925</v>
+      </c>
+      <c r="F6" s="6">
+        <f t="shared" si="1"/>
+        <v>0.18048780487804877</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -559,6 +827,10 @@
         <f t="shared" si="0"/>
         <v>325</v>
       </c>
+      <c r="F7" s="6">
+        <f t="shared" si="1"/>
+        <v>6.3414634146341464E-2</v>
+      </c>
     </row>
     <row r="8" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
@@ -566,7 +838,7 @@
       </c>
       <c r="B8" s="2">
         <f>SUM(B3:B7)</f>
-        <v>1650</v>
+        <v>1675</v>
       </c>
       <c r="C8" s="2">
         <f>SUM(C3:C7)</f>
@@ -574,14 +846,23 @@
       </c>
       <c r="D8" s="2">
         <f>SUM(D3:D7)</f>
-        <v>1550</v>
+        <v>1750</v>
+      </c>
+      <c r="E8" s="2">
+        <f t="shared" si="0"/>
+        <v>5125</v>
+      </c>
+      <c r="F8" s="7">
+        <f>SUM(F3:F7)</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="B8:D8" formulaRange="1"/>
+    <ignoredError sqref="B8:C8 D8" formulaRange="1"/>
+    <ignoredError sqref="E8" formula="1" formulaRange="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add minifs sheet in 13.monthly budget workbook
</commit_message>
<xml_diff>
--- a/13. Monthly Budget.xlsx
+++ b/13. Monthly Budget.xlsx
@@ -8,36 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\moin\Excel Practice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1DF3D26-6576-4E02-9371-B7A6E78175F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D285552-F437-4571-8193-BE80498F0A90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{0525C57C-F6D3-4E5A-BABF-0921013F3FE3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0525C57C-F6D3-4E5A-BABF-0921013F3FE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Monthly Budget " sheetId="3" r:id="rId1"/>
     <sheet name="Monthly Budget  (2)" sheetId="4" r:id="rId2"/>
+    <sheet name="MINIFS n MAXIFS" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="21">
   <si>
     <t>Bills</t>
   </si>
@@ -61,6 +51,45 @@
   </si>
   <si>
     <t>Percent</t>
+  </si>
+  <si>
+    <t>Donation</t>
+  </si>
+  <si>
+    <t>Person</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Saleem</t>
+  </si>
+  <si>
+    <t>Ayaan</t>
+  </si>
+  <si>
+    <t>Naman</t>
+  </si>
+  <si>
+    <t>Ayaan Total</t>
+  </si>
+  <si>
+    <t>Naman Total</t>
+  </si>
+  <si>
+    <t>Saleem Total</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Ayaan Min</t>
+  </si>
+  <si>
+    <t>Ayaan Max</t>
+  </si>
+  <si>
+    <t>Ayaan Sum</t>
   </si>
 </sst>
 </file>
@@ -68,8 +97,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="166" formatCode="mmm/yyyy"/>
-    <numFmt numFmtId="169" formatCode="mmm/dd/ddd/yyyy/mmm"/>
+    <numFmt numFmtId="164" formatCode="mmm/yyyy"/>
+    <numFmt numFmtId="165" formatCode="mmm/dd/ddd/yyyy/mmm"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -127,10 +156,10 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -454,240 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FF16D73-07B9-460A-92EB-0A055A3AA27D}">
-  <dimension ref="A2:O8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="10.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="11.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" style="1"/>
-    <col min="7" max="7" width="16.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:15" s="2" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="4">
-        <v>44562</v>
-      </c>
-      <c r="C2" s="4">
-        <v>44593</v>
-      </c>
-      <c r="D2" s="4">
-        <v>44621</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="3"/>
-    </row>
-    <row r="3" spans="1:15" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1">
-        <v>1000</v>
-      </c>
-      <c r="C3" s="1">
-        <v>1000</v>
-      </c>
-      <c r="D3" s="1">
-        <v>1000</v>
-      </c>
-      <c r="E3" s="2">
-        <f>SUM(B3:D3)</f>
-        <v>3000</v>
-      </c>
-      <c r="F3" s="1">
-        <f>E3/E$8</f>
-        <v>0.58536585365853655</v>
-      </c>
-      <c r="G3" s="5"/>
-    </row>
-    <row r="4" spans="1:15" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1">
-        <v>125</v>
-      </c>
-      <c r="C4" s="1">
-        <v>125</v>
-      </c>
-      <c r="D4" s="1">
-        <v>100</v>
-      </c>
-      <c r="E4" s="2">
-        <f t="shared" ref="E4:E8" si="0">SUM(B4:D4)</f>
-        <v>350</v>
-      </c>
-      <c r="F4" s="1">
-        <f t="shared" ref="F4:F7" si="1">E4/E$8</f>
-        <v>6.8292682926829273E-2</v>
-      </c>
-      <c r="I4" s="1">
-        <v>10</v>
-      </c>
-      <c r="J4" s="1">
-        <v>20</v>
-      </c>
-      <c r="M4" s="1">
-        <v>5</v>
-      </c>
-      <c r="N4" s="1">
-        <f>I$4*$M4</f>
-        <v>50</v>
-      </c>
-      <c r="O4" s="1">
-        <f>J$4*$M4</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1">
-        <v>150</v>
-      </c>
-      <c r="C5" s="1">
-        <v>200</v>
-      </c>
-      <c r="D5" s="1">
-        <v>175</v>
-      </c>
-      <c r="E5" s="2">
-        <f t="shared" si="0"/>
-        <v>525</v>
-      </c>
-      <c r="F5" s="1">
-        <f t="shared" si="1"/>
-        <v>0.1024390243902439</v>
-      </c>
-      <c r="M5" s="1">
-        <v>6</v>
-      </c>
-      <c r="N5" s="1">
-        <f t="shared" ref="N5:N7" si="2">I$4*$M5</f>
-        <v>60</v>
-      </c>
-      <c r="O5" s="1">
-        <f>J$4*$M5</f>
-        <v>120</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1">
-        <v>300</v>
-      </c>
-      <c r="C6" s="1">
-        <v>275</v>
-      </c>
-      <c r="D6" s="1">
-        <v>350</v>
-      </c>
-      <c r="E6" s="2">
-        <f t="shared" si="0"/>
-        <v>925</v>
-      </c>
-      <c r="F6" s="1">
-        <f t="shared" si="1"/>
-        <v>0.18048780487804877</v>
-      </c>
-      <c r="M6" s="1">
-        <v>7</v>
-      </c>
-      <c r="N6" s="1">
-        <f t="shared" si="2"/>
-        <v>70</v>
-      </c>
-      <c r="O6" s="1">
-        <f>J$4*$M6</f>
-        <v>140</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="1">
-        <v>100</v>
-      </c>
-      <c r="C7" s="1">
-        <v>100</v>
-      </c>
-      <c r="D7" s="1">
-        <v>125</v>
-      </c>
-      <c r="E7" s="2">
-        <f t="shared" si="0"/>
-        <v>325</v>
-      </c>
-      <c r="F7" s="1">
-        <f t="shared" si="1"/>
-        <v>6.3414634146341464E-2</v>
-      </c>
-      <c r="M7" s="1">
-        <v>8</v>
-      </c>
-      <c r="N7" s="1">
-        <f t="shared" si="2"/>
-        <v>80</v>
-      </c>
-      <c r="O7" s="1">
-        <f>J$4*$M7</f>
-        <v>160</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="2">
-        <f>SUM(B3:B7)</f>
-        <v>1675</v>
-      </c>
-      <c r="C8" s="2">
-        <f>SUM(C3:C7)</f>
-        <v>1700</v>
-      </c>
-      <c r="D8" s="2">
-        <f>SUM(D3:D7)</f>
-        <v>1750</v>
-      </c>
-      <c r="E8" s="2">
-        <f t="shared" si="0"/>
-        <v>5125</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="B8:D8" formulaRange="1"/>
-  </ignoredErrors>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C79055A-5DDB-4DD7-8258-797C0A05ECC1}">
   <dimension ref="A2:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:Q9"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -738,8 +537,8 @@
         <f>SUM(B3:D3)</f>
         <v>3000</v>
       </c>
-      <c r="F3" s="6">
-        <f>E3/$E$8</f>
+      <c r="F3" s="1">
+        <f>E3/E$8</f>
         <v>0.58536585365853655</v>
       </c>
       <c r="G3" s="5"/>
@@ -761,8 +560,8 @@
         <f t="shared" ref="E4:E8" si="0">SUM(B4:D4)</f>
         <v>350</v>
       </c>
-      <c r="F4" s="6">
-        <f t="shared" ref="F4:F7" si="1">E4/$E$8</f>
+      <c r="F4" s="1">
+        <f t="shared" ref="F4:F7" si="1">E4/E$8</f>
         <v>6.8292682926829273E-2</v>
       </c>
     </row>
@@ -783,7 +582,7 @@
         <f t="shared" si="0"/>
         <v>525</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="1">
         <f t="shared" si="1"/>
         <v>0.1024390243902439</v>
       </c>
@@ -805,7 +604,7 @@
         <f t="shared" si="0"/>
         <v>925</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="1">
         <f t="shared" si="1"/>
         <v>0.18048780487804877</v>
       </c>
@@ -827,7 +626,7 @@
         <f t="shared" si="0"/>
         <v>325</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="1">
         <f t="shared" si="1"/>
         <v>6.3414634146341464E-2</v>
       </c>
@@ -851,18 +650,478 @@
       <c r="E8" s="2">
         <f t="shared" si="0"/>
         <v>5125</v>
-      </c>
-      <c r="F8" s="7">
-        <f>SUM(F3:F7)</f>
-        <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="B8:C8 D8" formulaRange="1"/>
-    <ignoredError sqref="E8" formula="1" formulaRange="1"/>
+    <ignoredError sqref="B8:D8" formulaRange="1"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C79055A-5DDB-4DD7-8258-797C0A05ECC1}">
+  <dimension ref="A2:I8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:N16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="11.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="1"/>
+    <col min="7" max="7" width="16.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:9" s="2" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4">
+        <v>44562</v>
+      </c>
+      <c r="C2" s="4">
+        <v>44593</v>
+      </c>
+      <c r="D2" s="4">
+        <v>44621</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" spans="1:9" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1000</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1000</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E3" s="2">
+        <f>SUM(B3:D3)</f>
+        <v>3000</v>
+      </c>
+      <c r="F3" s="6">
+        <f>E3/$E$8</f>
+        <v>0.58536585365853655</v>
+      </c>
+      <c r="G3" s="5"/>
+      <c r="I3" s="7"/>
+    </row>
+    <row r="4" spans="1:9" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>125</v>
+      </c>
+      <c r="C4" s="1">
+        <v>125</v>
+      </c>
+      <c r="D4" s="1">
+        <v>100</v>
+      </c>
+      <c r="E4" s="2">
+        <f t="shared" ref="E4:E8" si="0">SUM(B4:D4)</f>
+        <v>350</v>
+      </c>
+      <c r="F4" s="6">
+        <f t="shared" ref="F4:F7" si="1">E4/$E$8</f>
+        <v>6.8292682926829273E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
+        <v>150</v>
+      </c>
+      <c r="C5" s="1">
+        <v>200</v>
+      </c>
+      <c r="D5" s="1">
+        <v>175</v>
+      </c>
+      <c r="E5" s="2">
+        <f t="shared" si="0"/>
+        <v>525</v>
+      </c>
+      <c r="F5" s="6">
+        <f t="shared" si="1"/>
+        <v>0.1024390243902439</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1">
+        <v>300</v>
+      </c>
+      <c r="C6" s="1">
+        <v>275</v>
+      </c>
+      <c r="D6" s="1">
+        <v>350</v>
+      </c>
+      <c r="E6" s="2">
+        <f t="shared" si="0"/>
+        <v>925</v>
+      </c>
+      <c r="F6" s="6">
+        <f t="shared" si="1"/>
+        <v>0.18048780487804877</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1">
+        <v>100</v>
+      </c>
+      <c r="C7" s="1">
+        <v>100</v>
+      </c>
+      <c r="D7" s="1">
+        <v>125</v>
+      </c>
+      <c r="E7" s="2">
+        <f t="shared" si="0"/>
+        <v>325</v>
+      </c>
+      <c r="F7" s="6">
+        <f t="shared" si="1"/>
+        <v>6.3414634146341464E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2">
+        <f>SUM(B$3:B$7)</f>
+        <v>1675</v>
+      </c>
+      <c r="C8" s="2">
+        <f t="shared" ref="C8:D8" si="2">SUM(C$3:C$7)</f>
+        <v>1700</v>
+      </c>
+      <c r="D8" s="2">
+        <f t="shared" si="2"/>
+        <v>1750</v>
+      </c>
+      <c r="E8" s="2">
+        <f t="shared" si="0"/>
+        <v>5125</v>
+      </c>
+      <c r="F8" s="7">
+        <f>SUM(F3:F7)</f>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDB58E34-8B72-4003-899B-111F504A93AF}">
+  <dimension ref="A1:E19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="2" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+    </row>
+    <row r="2" spans="1:5" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>500</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="1">
+        <f>_xlfn.MINIFS($A$2:$A$18,$B$2:$B$18,"Ayaan")</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>900</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="1">
+        <f>_xlfn.MAXIFS($A$2:$A$18,$B$2:$B$18,"Ayaan")</f>
+        <v>5900</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>5900</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="1">
+        <f>SUMIFS($A$2:$A$18,$B$2:$B$18,"Ayaan")</f>
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>700</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <f>SUBTOTAL(9,A2:A5)</f>
+        <v>8000</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>450</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="1">
+        <f>_xlfn.MINIFS($A$2:$A$18,$B$2:$B$18,"Naman")</f>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>200</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="1">
+        <f>_xlfn.MAXIFS($A$2:$A$18,$B$2:$B$18,"Naman")</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>500</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="1">
+        <f>SUMIFS($A$2:$A$18,$B$2:$B$18,"Naman")</f>
+        <v>1340</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>90</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>100</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <f>SUBTOTAL(9,A7:A11)</f>
+        <v>1340</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:5" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>1000</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="1">
+        <f>_xlfn.MINIFS($A$2:$A$18,$B$2:$B$18,"Saleem")</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>1500</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="1">
+        <f>_xlfn.MAXIFS($A$2:$A$18,$B$2:$B$18,"Saleem")</f>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>3000</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" s="1">
+        <f>SUMIFS($A$2:$A$18,$B$2:$B$18,"Saleem")</f>
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>500</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>1000</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <f>SUBTOTAL(9,A13:A17)</f>
+        <v>7000</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <f>SUBTOTAL(9,A2:A17)</f>
+        <v>16340</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C17">
+    <sortCondition ref="B2:B17"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>